<commit_message>
Updates to metadata and scripts.
</commit_message>
<xml_diff>
--- a/data/RNAseq Variants of Interest List_V2.xlsx
+++ b/data/RNAseq Variants of Interest List_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shutchens/Documents/Git-Repos/mecfs-dge-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B5CF83-621D-9D4E-8A43-9EC0C111DF4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36B0841B-90EB-2946-8EFF-3CE2A761C25D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41340" yWindow="4360" windowWidth="31920" windowHeight="19280" xr2:uid="{3932C719-71D1-B14D-983B-870F2D8EB1AB}"/>
+    <workbookView minimized="1" xWindow="-47100" yWindow="5520" windowWidth="31920" windowHeight="14840" xr2:uid="{3932C719-71D1-B14D-983B-870F2D8EB1AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -787,19 +787,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1119,19 +1118,17 @@
   <dimension ref="A1:J84"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection sqref="A1:J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.83203125" style="6"/>
-    <col min="5" max="5" width="21.83203125" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15" style="6" customWidth="1"/>
-    <col min="7" max="7" width="43.83203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="57.5" style="6" customWidth="1"/>
-    <col min="9" max="9" width="44" style="6" customWidth="1"/>
-    <col min="10" max="16384" width="10.83203125" style="6"/>
+    <col min="1" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="7" max="7" width="43.83203125" customWidth="1"/>
+    <col min="8" max="8" width="57.5" customWidth="1"/>
+    <col min="9" max="9" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" ht="18" x14ac:dyDescent="0.2">
@@ -1191,7 +1188,7 @@
       <c r="H2" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" t="s">
         <v>76</v>
       </c>
       <c r="J2" s="4" t="s">
@@ -1223,7 +1220,7 @@
       <c r="H3" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" t="s">
         <v>79</v>
       </c>
       <c r="J3" s="4" t="s">
@@ -1255,7 +1252,7 @@
       <c r="H4" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" t="s">
         <v>81</v>
       </c>
       <c r="J4" s="4" t="s">
@@ -1340,7 +1337,7 @@
       <c r="H7" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" t="s">
         <v>85</v>
       </c>
       <c r="J7" s="4" t="s">
@@ -3519,7 +3516,7 @@
       <c r="G77" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="H77" s="7" t="s">
+      <c r="H77" s="6" t="s">
         <v>178</v>
       </c>
       <c r="I77" s="4" t="s">
@@ -3583,7 +3580,7 @@
       <c r="G79" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="H79" s="7" t="s">
+      <c r="H79" s="6" t="s">
         <v>178</v>
       </c>
       <c r="I79" s="4" t="s">
@@ -3647,7 +3644,7 @@
       <c r="G81" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="H81" s="7" t="s">
+      <c r="H81" s="6" t="s">
         <v>178</v>
       </c>
       <c r="I81" s="4" t="s">

</xml_diff>